<commit_message>
More stocks added to SelMat
</commit_message>
<xml_diff>
--- a/selectivity/SelMat.xlsx
+++ b/selectivity/SelMat.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>diffA50</t>
   </si>
@@ -72,13 +72,28 @@
     <t>Fbar</t>
   </si>
   <si>
-    <t>Selection range is the number of years between A25 and A75 - indicates the steepness of the selectivity curve</t>
-  </si>
-  <si>
     <t>Georges Bank</t>
   </si>
   <si>
     <t>2007-2016</t>
+  </si>
+  <si>
+    <t>Selection range' is the number of years between A25 and A75 - indicates the steepness of the selectivity curve</t>
+  </si>
+  <si>
+    <t>Greenland</t>
+  </si>
+  <si>
+    <t>NAFO 3M</t>
+  </si>
+  <si>
+    <t>NAFO 3NO</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Celtic</t>
   </si>
 </sst>
 </file>
@@ -122,9 +137,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -687,6 +703,323 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000007-59CD-461D-B816-CD86BD6B3BD7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:v>Greenland</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.67400000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D8B2-41E9-8561-A0075C175C4B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:v>NAFO 3M</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7.9000000000000001E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D8B2-41E9-8561-A0075C175C4B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:v>NAFO 3NO</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-2.67</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7.5999999999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D8B2-41E9-8561-A0075C175C4B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:v>Norway</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-0.34</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.25700000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-D8B2-41E9-8561-A0075C175C4B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:tx>
+            <c:v>Celtic</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-0.19</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.71199999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-D8B2-41E9-8561-A0075C175C4B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1555,15 +1888,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1162050</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>1152525</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1848,10 +2181,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2004,7 +2337,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1">
         <v>0.71</v>
@@ -2045,7 +2378,7 @@
         <v>1.07</v>
       </c>
       <c r="G8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2071,9 +2404,124 @@
         <v>15</v>
       </c>
     </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="C10">
+        <v>4.32</v>
+      </c>
+      <c r="D10">
+        <v>4.62</v>
+      </c>
+      <c r="E10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F10">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="G10" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C11">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D11">
+        <v>4.38</v>
+      </c>
+      <c r="E11">
+        <v>1.82</v>
+      </c>
+      <c r="F11">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1">
+        <v>-2.67</v>
+      </c>
+      <c r="C12">
+        <v>5.51</v>
+      </c>
+      <c r="D12">
+        <v>2.84</v>
+      </c>
+      <c r="E12">
+        <v>0.74</v>
+      </c>
+      <c r="F12">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1">
+        <v>-0.34</v>
+      </c>
+      <c r="C13">
+        <v>5.29</v>
+      </c>
+      <c r="D13">
+        <v>4.95</v>
+      </c>
+      <c r="E13">
+        <v>2.11</v>
+      </c>
+      <c r="F13">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="G13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="1">
+        <v>-0.19</v>
+      </c>
+      <c r="C14">
+        <v>2.02</v>
+      </c>
+      <c r="D14">
+        <v>2.21</v>
+      </c>
+      <c r="E14">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="F14">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="G14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock status added in SelMat.xls
</commit_message>
<xml_diff>
--- a/selectivity/SelMat.xlsx
+++ b/selectivity/SelMat.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>diffA50</t>
   </si>
@@ -94,6 +94,15 @@
   </si>
   <si>
     <t>Celtic</t>
+  </si>
+  <si>
+    <t>Exploitation status</t>
+  </si>
+  <si>
+    <t>Stock status</t>
+  </si>
+  <si>
+    <t>Stocks above the red dashed line are overexploited</t>
   </si>
 </sst>
 </file>
@@ -117,12 +126,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -137,10 +158,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1934,6 +1957,56 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Connector 8"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2162175" y="5895976"/>
+          <a:ext cx="3028950" cy="9524"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2200,10 +2273,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2214,9 +2287,11 @@
     <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2238,8 +2313,14 @@
       <c r="G1" t="s">
         <v>2</v>
       </c>
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2261,8 +2342,10 @@
       <c r="G2" t="s">
         <v>3</v>
       </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2284,8 +2367,10 @@
       <c r="G3" t="s">
         <v>3</v>
       </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2307,8 +2392,10 @@
       <c r="G4" t="s">
         <v>3</v>
       </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2330,8 +2417,10 @@
       <c r="G5" t="s">
         <v>3</v>
       </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2353,8 +2442,10 @@
       <c r="G6" t="s">
         <v>3</v>
       </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -2376,8 +2467,10 @@
       <c r="G7" t="s">
         <v>12</v>
       </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -2399,8 +2492,10 @@
       <c r="G8" t="s">
         <v>18</v>
       </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2422,8 +2517,9 @@
       <c r="G9" t="s">
         <v>15</v>
       </c>
+      <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -2445,8 +2541,10 @@
       <c r="G10" t="s">
         <v>3</v>
       </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -2468,8 +2566,9 @@
       <c r="G11" t="s">
         <v>3</v>
       </c>
+      <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -2491,8 +2590,9 @@
       <c r="G12" t="s">
         <v>3</v>
       </c>
+      <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -2515,7 +2615,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2537,10 +2637,17 @@
       <c r="G14" t="s">
         <v>3</v>
       </c>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>